<commit_message>
pdf creation extra column and empty row
</commit_message>
<xml_diff>
--- a/SecondHalf/SecondHalf/FinalResult.xlsx
+++ b/SecondHalf/SecondHalf/FinalResult.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72b64a486f66b2e3/Documents/UiPath/.repositories/RPA-PasswordManager/SecondHalf/SecondHalf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laur\Desktop\RPA\proiect\RPA-PasswordManager\SecondHalf\SecondHalf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC10481C31584CE85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD27BD6-B480-4D4F-9BFE-C5163D3AEE73}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DBACAD-7010-433B-8353-8F216032B0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,62 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>nume site</t>
-  </si>
-  <si>
-    <t>emag</t>
-  </si>
-  <si>
-    <t>facebook</t>
-  </si>
-  <si>
-    <t>youtube</t>
-  </si>
-  <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>Netflix</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>andreiEmaaaaaaaag</t>
-  </si>
-  <si>
-    <t>andreiFb</t>
-  </si>
-  <si>
-    <t>andreiYT</t>
-  </si>
-  <si>
-    <t>andreiGgl</t>
-  </si>
-  <si>
-    <t>andreiNTFLX</t>
-  </si>
-  <si>
-    <t>parola noua</t>
-  </si>
-  <si>
-    <t>parolaEmag</t>
-  </si>
-  <si>
-    <t>parolaFb</t>
-  </si>
-  <si>
-    <t>parolaYTB</t>
-  </si>
-  <si>
-    <t>parolaGGL</t>
-  </si>
-  <si>
-    <t>parolaNTFL</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,81 +345,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
check mail headers, repair pdfs, loop through mails
</commit_message>
<xml_diff>
--- a/SecondHalf/SecondHalf/FinalResult.xlsx
+++ b/SecondHalf/SecondHalf/FinalResult.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72b64a486f66b2e3/Documents/UiPath/.repositories/RPA-PasswordManager/SecondHalf/SecondHalf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laur\Desktop\RPA\proiect\RPA-PasswordManager\SecondHalf\SecondHalf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{63DBACAD-7010-433B-8353-8F216032B0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BBB796-9749-41CE-959F-271CB2F5B540}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE87EF9-2415-43B2-95A9-D9C117F41BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="1845" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,65 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>nume site</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>parola noua</t>
-  </si>
-  <si>
-    <t>mailFound</t>
-  </si>
-  <si>
-    <t>emag</t>
-  </si>
-  <si>
-    <t>facebook</t>
-  </si>
-  <si>
-    <t>youtube</t>
-  </si>
-  <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>Netflix</t>
-  </si>
-  <si>
-    <t>andreiEmaaaaaaaag</t>
-  </si>
-  <si>
-    <t>andreiFb</t>
-  </si>
-  <si>
-    <t>andreiYT</t>
-  </si>
-  <si>
-    <t>andreiGgl</t>
-  </si>
-  <si>
-    <t>andreiNTFLX</t>
-  </si>
-  <si>
-    <t>parolaEmag</t>
-  </si>
-  <si>
-    <t>parolaFb</t>
-  </si>
-  <si>
-    <t>parolaYTB</t>
-  </si>
-  <si>
-    <t>parolaGGL</t>
-  </si>
-  <si>
-    <t>parolaNTFL</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,99 +345,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>